<commit_message>
Updated csv files and added all countries to the lookup table
</commit_message>
<xml_diff>
--- a/International.xlsx
+++ b/International.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="0" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="0" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\GitHub\D3Playground\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="270" yWindow="585" windowWidth="12135" windowHeight="9660"/>
   </bookViews>
@@ -158,9 +163,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -170,6 +177,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -218,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,7 +476,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -474,7 +484,7 @@
     <col min="1" max="1" width="11.28515625"/>
     <col min="2" max="2" width="10.28515625"/>
     <col min="3" max="3" width="13.140625"/>
-    <col min="4" max="4" width="10.28515625"/>
+    <col min="4" max="4" width="10.28515625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -487,7 +497,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -501,7 +511,7 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>117</v>
       </c>
     </row>
@@ -515,7 +525,7 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>150000</v>
       </c>
     </row>
@@ -529,7 +539,7 @@
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>258666.62</v>
       </c>
     </row>
@@ -543,7 +553,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>115</v>
       </c>
     </row>
@@ -557,7 +567,7 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>185135.37</v>
       </c>
     </row>
@@ -571,7 +581,7 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>300</v>
       </c>
     </row>
@@ -585,7 +595,7 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>116</v>
       </c>
     </row>
@@ -599,7 +609,7 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>83502.460000000006</v>
       </c>
     </row>
@@ -613,7 +623,7 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>25</v>
       </c>
     </row>
@@ -627,7 +637,7 @@
       <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>512185</v>
       </c>
     </row>
@@ -641,7 +651,7 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>120</v>
       </c>
     </row>
@@ -655,7 +665,7 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>100</v>
       </c>
     </row>
@@ -669,7 +679,7 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>21.93</v>
       </c>
     </row>
@@ -683,7 +693,7 @@
       <c r="C15">
         <v>0</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>26409.599999999999</v>
       </c>
     </row>
@@ -697,7 +707,7 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>3145.88</v>
       </c>
     </row>
@@ -711,7 +721,7 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>286400</v>
       </c>
     </row>
@@ -725,7 +735,7 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>40</v>
       </c>
     </row>
@@ -739,7 +749,7 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>10</v>
       </c>
     </row>
@@ -753,7 +763,7 @@
       <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>250</v>
       </c>
     </row>
@@ -767,7 +777,7 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>25</v>
       </c>
     </row>
@@ -781,7 +791,7 @@
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>50</v>
       </c>
     </row>
@@ -795,7 +805,7 @@
       <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>11170.75</v>
       </c>
     </row>
@@ -809,7 +819,7 @@
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>568250</v>
       </c>
     </row>
@@ -823,7 +833,7 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>50</v>
       </c>
     </row>
@@ -837,7 +847,7 @@
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <v>3800</v>
       </c>
     </row>

</xml_diff>